<commit_message>
Update 1.4 IPA Tag 2
Changelog:
- Planung des Grundschutzstufen-Konzepts abgeschlossen
- Planung des Approval-Meetings abgeschlossen
- Mit der Planung des Testkonzepts begonnen
</commit_message>
<xml_diff>
--- a/02_Zeitplanung_Nideröst.xlsx
+++ b/02_Zeitplanung_Nideröst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IPA_Nideröst_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B24C7A9-A288-4AB7-8B18-66539C08F954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F716FA-A914-4AC3-9B6E-18291041CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" xr2:uid="{8796DB52-94B7-4869-AF39-88ED6CB3CCF9}"/>
   </bookViews>
@@ -201,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +243,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF008080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -818,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -873,25 +880,38 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -906,14 +926,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -921,29 +953,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -963,51 +1007,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1334,8 +1342,8 @@
   </sheetPr>
   <dimension ref="B1:CF84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,120 +1355,120 @@
   <sheetData>
     <row r="1" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="87">
         <v>45376</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="40">
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="87">
         <v>45377</v>
       </c>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="40">
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="87">
         <v>45378</v>
       </c>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="40">
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="85"/>
+      <c r="Y2" s="85"/>
+      <c r="Z2" s="85"/>
+      <c r="AA2" s="85"/>
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="87">
         <v>45384</v>
       </c>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="41"/>
-      <c r="AI2" s="41"/>
-      <c r="AJ2" s="42"/>
-      <c r="AK2" s="40">
+      <c r="AD2" s="85"/>
+      <c r="AE2" s="85"/>
+      <c r="AF2" s="85"/>
+      <c r="AG2" s="85"/>
+      <c r="AH2" s="85"/>
+      <c r="AI2" s="85"/>
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="87">
         <v>45385</v>
       </c>
-      <c r="AL2" s="41"/>
-      <c r="AM2" s="41"/>
-      <c r="AN2" s="41"/>
-      <c r="AO2" s="41"/>
-      <c r="AP2" s="41"/>
-      <c r="AQ2" s="41"/>
-      <c r="AR2" s="42"/>
-      <c r="AS2" s="40">
+      <c r="AL2" s="85"/>
+      <c r="AM2" s="85"/>
+      <c r="AN2" s="85"/>
+      <c r="AO2" s="85"/>
+      <c r="AP2" s="85"/>
+      <c r="AQ2" s="85"/>
+      <c r="AR2" s="86"/>
+      <c r="AS2" s="87">
         <v>45387</v>
       </c>
-      <c r="AT2" s="41"/>
-      <c r="AU2" s="41"/>
-      <c r="AV2" s="41"/>
-      <c r="AW2" s="41"/>
-      <c r="AX2" s="41"/>
-      <c r="AY2" s="41"/>
-      <c r="AZ2" s="42"/>
-      <c r="BA2" s="40">
+      <c r="AT2" s="85"/>
+      <c r="AU2" s="85"/>
+      <c r="AV2" s="85"/>
+      <c r="AW2" s="85"/>
+      <c r="AX2" s="85"/>
+      <c r="AY2" s="85"/>
+      <c r="AZ2" s="86"/>
+      <c r="BA2" s="87">
         <v>45390</v>
       </c>
-      <c r="BB2" s="41"/>
-      <c r="BC2" s="41"/>
-      <c r="BD2" s="41"/>
-      <c r="BE2" s="41"/>
-      <c r="BF2" s="41"/>
-      <c r="BG2" s="41"/>
-      <c r="BH2" s="41"/>
-      <c r="BI2" s="40">
+      <c r="BB2" s="85"/>
+      <c r="BC2" s="85"/>
+      <c r="BD2" s="85"/>
+      <c r="BE2" s="85"/>
+      <c r="BF2" s="85"/>
+      <c r="BG2" s="85"/>
+      <c r="BH2" s="85"/>
+      <c r="BI2" s="87">
         <v>45391</v>
       </c>
-      <c r="BJ2" s="41"/>
-      <c r="BK2" s="41"/>
-      <c r="BL2" s="41"/>
-      <c r="BM2" s="41"/>
-      <c r="BN2" s="41"/>
-      <c r="BO2" s="41"/>
-      <c r="BP2" s="42"/>
-      <c r="BQ2" s="41">
+      <c r="BJ2" s="85"/>
+      <c r="BK2" s="85"/>
+      <c r="BL2" s="85"/>
+      <c r="BM2" s="85"/>
+      <c r="BN2" s="85"/>
+      <c r="BO2" s="85"/>
+      <c r="BP2" s="86"/>
+      <c r="BQ2" s="85">
         <v>45392</v>
       </c>
-      <c r="BR2" s="41"/>
-      <c r="BS2" s="41"/>
-      <c r="BT2" s="41"/>
-      <c r="BU2" s="41"/>
-      <c r="BV2" s="41"/>
-      <c r="BW2" s="41"/>
-      <c r="BX2" s="42"/>
-      <c r="BY2" s="40">
+      <c r="BR2" s="85"/>
+      <c r="BS2" s="85"/>
+      <c r="BT2" s="85"/>
+      <c r="BU2" s="85"/>
+      <c r="BV2" s="85"/>
+      <c r="BW2" s="85"/>
+      <c r="BX2" s="86"/>
+      <c r="BY2" s="87">
         <v>45394</v>
       </c>
-      <c r="BZ2" s="41"/>
-      <c r="CA2" s="41"/>
-      <c r="CB2" s="41"/>
-      <c r="CC2" s="41"/>
-      <c r="CD2" s="41"/>
-      <c r="CE2" s="41"/>
-      <c r="CF2" s="42"/>
+      <c r="BZ2" s="85"/>
+      <c r="CA2" s="85"/>
+      <c r="CB2" s="85"/>
+      <c r="CC2" s="85"/>
+      <c r="CD2" s="85"/>
+      <c r="CE2" s="85"/>
+      <c r="CF2" s="86"/>
     </row>
     <row r="3" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="93"/>
       <c r="E3" s="25" t="s">
         <v>2</v>
       </c>
@@ -1703,9 +1711,9 @@
       </c>
     </row>
     <row r="4" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="69"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
@@ -1948,10 +1956,10 @@
       </c>
     </row>
     <row r="5" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="57"/>
+      <c r="C5" s="96"/>
       <c r="D5" s="12"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
@@ -2035,17 +2043,17 @@
       <c r="CF5" s="24"/>
     </row>
     <row r="6" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="51">
+      <c r="B6" s="71">
         <v>1</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="88" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="70"/>
-      <c r="F6" s="71"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2126,13 +2134,13 @@
       <c r="CF6" s="3"/>
     </row>
     <row r="7" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="52"/>
-      <c r="C7" s="59"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="87"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2213,10 +2221,10 @@
       <c r="CF7" s="3"/>
     </row>
     <row r="8" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="60">
+      <c r="B8" s="62">
         <v>2</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="77" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -2224,8 +2232,8 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -2304,14 +2312,14 @@
       <c r="CF8" s="3"/>
     </row>
     <row r="9" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="52"/>
-      <c r="C9" s="63"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="81"/>
       <c r="D9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="87"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2391,10 +2399,10 @@
       <c r="CF9" s="3"/>
     </row>
     <row r="10" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="60">
+      <c r="B10" s="62">
         <v>3</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="77" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -2404,7 +2412,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="71"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="3"/>
@@ -2482,16 +2490,16 @@
       <c r="CF10" s="3"/>
     </row>
     <row r="11" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="53"/>
-      <c r="C11" s="62"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="3"/>
@@ -2569,10 +2577,10 @@
       <c r="CF11" s="3"/>
     </row>
     <row r="12" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="48"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="8" t="s">
         <v>4</v>
       </c>
@@ -2580,7 +2588,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="71"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="22"/>
       <c r="K12" s="15"/>
       <c r="L12" s="20"/>
@@ -2658,8 +2666,8 @@
       <c r="CF12" s="20"/>
     </row>
     <row r="13" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="49"/>
-      <c r="C13" s="50"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="9" t="s">
         <v>5</v>
       </c>
@@ -2667,7 +2675,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="87"/>
+      <c r="I13" s="54"/>
       <c r="J13" s="22"/>
       <c r="K13" s="15"/>
       <c r="L13" s="20"/>
@@ -2832,10 +2840,10 @@
       <c r="CF14" s="21"/>
     </row>
     <row r="15" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="51">
+      <c r="B15" s="71">
         <v>4</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="88" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -2846,8 +2854,8 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
       <c r="L15" s="3"/>
       <c r="M15" s="4"/>
       <c r="N15" s="1"/>
@@ -2923,8 +2931,8 @@
       <c r="CF15" s="3"/>
     </row>
     <row r="16" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="52"/>
-      <c r="C16" s="59"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="6" t="s">
         <v>5</v>
       </c>
@@ -2933,7 +2941,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="87"/>
+      <c r="J16" s="54"/>
       <c r="K16" s="1"/>
       <c r="L16" s="3"/>
       <c r="M16" s="4"/>
@@ -3010,10 +3018,10 @@
       <c r="CF16" s="3"/>
     </row>
     <row r="17" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="60">
+      <c r="B17" s="62">
         <v>5</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="77" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -3026,7 +3034,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="72"/>
+      <c r="L17" s="42"/>
       <c r="M17" s="4"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -3101,8 +3109,8 @@
       <c r="CF17" s="3"/>
     </row>
     <row r="18" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="52"/>
-      <c r="C18" s="63"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="6" t="s">
         <v>5</v>
       </c>
@@ -3112,7 +3120,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="87"/>
+      <c r="K18" s="54"/>
       <c r="L18" s="3"/>
       <c r="M18" s="4"/>
       <c r="N18" s="1"/>
@@ -3188,10 +3196,10 @@
       <c r="CF18" s="3"/>
     </row>
     <row r="19" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="60">
+      <c r="B19" s="62">
         <v>6</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="77" t="s">
         <v>52</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -3205,11 +3213,11 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="70"/>
-      <c r="N19" s="71"/>
-      <c r="O19" s="71"/>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="92"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="3"/>
@@ -3279,8 +3287,8 @@
       <c r="CF19" s="3"/>
     </row>
     <row r="20" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="52"/>
-      <c r="C20" s="63"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="6" t="s">
         <v>5</v>
       </c>
@@ -3291,12 +3299,12 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="98"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="3"/>
@@ -3366,7 +3374,7 @@
       <c r="CF20" s="3"/>
     </row>
     <row r="21" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="60">
+      <c r="B21" s="62">
         <v>7</v>
       </c>
       <c r="C21" s="73" t="s">
@@ -3387,8 +3395,8 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="71"/>
-      <c r="R21" s="71"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
       <c r="S21" s="1"/>
       <c r="T21" s="3"/>
       <c r="U21" s="4"/>
@@ -3457,8 +3465,8 @@
       <c r="CF21" s="3"/>
     </row>
     <row r="22" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="52"/>
-      <c r="C22" s="55"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="76"/>
       <c r="D22" s="6" t="s">
         <v>5</v>
       </c>
@@ -3475,8 +3483,8 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
       <c r="T22" s="3"/>
       <c r="U22" s="4"/>
       <c r="V22" s="1"/>
@@ -3544,10 +3552,10 @@
       <c r="CF22" s="3"/>
     </row>
     <row r="23" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="60">
+      <c r="B23" s="62">
         <v>8</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="79" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -3567,13 +3575,12 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="71"/>
-      <c r="T23" s="72"/>
-      <c r="U23" s="70"/>
-      <c r="V23" s="71"/>
-      <c r="W23" s="71"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="42"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="41"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="3"/>
@@ -3635,8 +3642,8 @@
       <c r="CF23" s="3"/>
     </row>
     <row r="24" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="53"/>
-      <c r="C24" s="58"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="7" t="s">
         <v>5</v>
       </c>
@@ -3655,7 +3662,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="3"/>
+      <c r="T24" s="59"/>
       <c r="U24" s="4"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
@@ -3722,10 +3729,10 @@
       <c r="CF24" s="3"/>
     </row>
     <row r="25" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="48"/>
+      <c r="C25" s="65"/>
       <c r="D25" s="8" t="s">
         <v>4</v>
       </c>
@@ -3747,7 +3754,7 @@
       <c r="T25" s="20"/>
       <c r="U25" s="18"/>
       <c r="V25" s="15"/>
-      <c r="W25" s="71"/>
+      <c r="W25" s="41"/>
       <c r="X25" s="15"/>
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
@@ -3811,8 +3818,8 @@
       <c r="CF25" s="20"/>
     </row>
     <row r="26" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="49"/>
-      <c r="C26" s="50"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="67"/>
       <c r="D26" s="9" t="s">
         <v>5</v>
       </c>
@@ -3898,7 +3905,7 @@
       <c r="CF26" s="20"/>
     </row>
     <row r="27" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="94"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="11" t="s">
         <v>10</v>
       </c>
@@ -3985,10 +3992,10 @@
       <c r="CF27" s="21"/>
     </row>
     <row r="28" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="96">
+      <c r="B28" s="82">
         <v>9</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="77" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -4012,9 +4019,9 @@
       <c r="T28" s="3"/>
       <c r="U28" s="4"/>
       <c r="V28" s="1"/>
-      <c r="W28" s="71"/>
-      <c r="X28" s="71"/>
-      <c r="Y28" s="71"/>
+      <c r="W28" s="97"/>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="41"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="3"/>
@@ -4076,8 +4083,8 @@
       <c r="CF28" s="3"/>
     </row>
     <row r="29" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="97"/>
-      <c r="C29" s="62"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="7" t="s">
         <v>5</v>
       </c>
@@ -4163,10 +4170,10 @@
       <c r="CF29" s="3"/>
     </row>
     <row r="30" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="95">
+      <c r="B30" s="84">
         <v>10</v>
       </c>
-      <c r="C30" s="61" t="s">
+      <c r="C30" s="77" t="s">
         <v>47</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -4193,8 +4200,8 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
-      <c r="Z30" s="71"/>
-      <c r="AA30" s="71"/>
+      <c r="Z30" s="41"/>
+      <c r="AA30" s="41"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="4"/>
       <c r="AD30" s="1"/>
@@ -4254,8 +4261,8 @@
       <c r="CF30" s="3"/>
     </row>
     <row r="31" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="52"/>
-      <c r="C31" s="63"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="81"/>
       <c r="D31" s="6" t="s">
         <v>5</v>
       </c>
@@ -4341,10 +4348,10 @@
       <c r="CF31" s="3"/>
     </row>
     <row r="32" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="60">
+      <c r="B32" s="62">
         <v>11</v>
       </c>
-      <c r="C32" s="61" t="s">
+      <c r="C32" s="77" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -4373,9 +4380,9 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
-      <c r="AB32" s="72"/>
-      <c r="AC32" s="70"/>
-      <c r="AD32" s="71"/>
+      <c r="AB32" s="42"/>
+      <c r="AC32" s="40"/>
+      <c r="AD32" s="41"/>
       <c r="AE32" s="1"/>
       <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
@@ -4432,8 +4439,8 @@
       <c r="CF32" s="3"/>
     </row>
     <row r="33" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="53"/>
-      <c r="C33" s="62"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="78"/>
       <c r="D33" s="7" t="s">
         <v>5</v>
       </c>
@@ -4519,10 +4526,10 @@
       <c r="CF33" s="3"/>
     </row>
     <row r="34" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="48"/>
+      <c r="C34" s="65"/>
       <c r="D34" s="8" t="s">
         <v>4</v>
       </c>
@@ -4551,7 +4558,7 @@
       <c r="AA34" s="15"/>
       <c r="AB34" s="20"/>
       <c r="AC34" s="18"/>
-      <c r="AD34" s="71"/>
+      <c r="AD34" s="41"/>
       <c r="AE34" s="15"/>
       <c r="AF34" s="15"/>
       <c r="AG34" s="15"/>
@@ -4608,8 +4615,8 @@
       <c r="CF34" s="20"/>
     </row>
     <row r="35" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="49"/>
-      <c r="C35" s="50"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="67"/>
       <c r="D35" s="9" t="s">
         <v>5</v>
       </c>
@@ -4782,10 +4789,10 @@
       <c r="CF36" s="21"/>
     </row>
     <row r="37" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="51">
+      <c r="B37" s="71">
         <v>12</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="78" t="s">
         <v>50</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -4816,8 +4823,8 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="3"/>
       <c r="AC37" s="4"/>
-      <c r="AD37" s="71"/>
-      <c r="AE37" s="71"/>
+      <c r="AD37" s="41"/>
+      <c r="AE37" s="41"/>
       <c r="AF37" s="1"/>
       <c r="AG37" s="1"/>
       <c r="AH37" s="1"/>
@@ -4873,8 +4880,8 @@
       <c r="CF37" s="3"/>
     </row>
     <row r="38" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="52"/>
-      <c r="C38" s="63"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="81"/>
       <c r="D38" s="6" t="s">
         <v>5</v>
       </c>
@@ -4960,10 +4967,10 @@
       <c r="CF38" s="3"/>
     </row>
     <row r="39" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="60">
+      <c r="B39" s="62">
         <v>13</v>
       </c>
-      <c r="C39" s="61" t="s">
+      <c r="C39" s="77" t="s">
         <v>30</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -4996,8 +5003,8 @@
       <c r="AC39" s="4"/>
       <c r="AD39" s="1"/>
       <c r="AE39" s="1"/>
-      <c r="AF39" s="71"/>
-      <c r="AG39" s="71"/>
+      <c r="AF39" s="41"/>
+      <c r="AG39" s="41"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
       <c r="AJ39" s="3"/>
@@ -5051,8 +5058,8 @@
       <c r="CF39" s="3"/>
     </row>
     <row r="40" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="52"/>
-      <c r="C40" s="63"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="81"/>
       <c r="D40" s="6" t="s">
         <v>5</v>
       </c>
@@ -5138,10 +5145,10 @@
       <c r="CF40" s="3"/>
     </row>
     <row r="41" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B41" s="60">
+      <c r="B41" s="62">
         <v>14</v>
       </c>
-      <c r="C41" s="74" t="s">
+      <c r="C41" s="79" t="s">
         <v>31</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -5176,10 +5183,10 @@
       <c r="AE41" s="1"/>
       <c r="AF41" s="1"/>
       <c r="AG41" s="1"/>
-      <c r="AH41" s="71"/>
-      <c r="AI41" s="71"/>
-      <c r="AJ41" s="72"/>
-      <c r="AK41" s="70"/>
+      <c r="AH41" s="41"/>
+      <c r="AI41" s="41"/>
+      <c r="AJ41" s="42"/>
+      <c r="AK41" s="40"/>
       <c r="AL41" s="1"/>
       <c r="AM41" s="1"/>
       <c r="AN41" s="1"/>
@@ -5229,8 +5236,8 @@
       <c r="CF41" s="3"/>
     </row>
     <row r="42" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B42" s="52"/>
-      <c r="C42" s="59"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="80"/>
       <c r="D42" s="6" t="s">
         <v>5</v>
       </c>
@@ -5316,10 +5323,10 @@
       <c r="CF42" s="3"/>
     </row>
     <row r="43" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B43" s="60">
+      <c r="B43" s="62">
         <v>15</v>
       </c>
-      <c r="C43" s="61" t="s">
+      <c r="C43" s="77" t="s">
         <v>32</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -5358,15 +5365,15 @@
       <c r="AI43" s="1"/>
       <c r="AJ43" s="3"/>
       <c r="AK43" s="4"/>
-      <c r="AL43" s="71"/>
-      <c r="AM43" s="71"/>
-      <c r="AN43" s="71"/>
-      <c r="AO43" s="71"/>
-      <c r="AP43" s="71"/>
-      <c r="AQ43" s="71"/>
-      <c r="AR43" s="72"/>
-      <c r="AS43" s="70"/>
-      <c r="AT43" s="71"/>
+      <c r="AL43" s="41"/>
+      <c r="AM43" s="41"/>
+      <c r="AN43" s="41"/>
+      <c r="AO43" s="41"/>
+      <c r="AP43" s="41"/>
+      <c r="AQ43" s="41"/>
+      <c r="AR43" s="42"/>
+      <c r="AS43" s="40"/>
+      <c r="AT43" s="41"/>
       <c r="AU43" s="1"/>
       <c r="AV43" s="1"/>
       <c r="AW43" s="1"/>
@@ -5407,8 +5414,8 @@
       <c r="CF43" s="3"/>
     </row>
     <row r="44" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B44" s="52"/>
-      <c r="C44" s="63"/>
+      <c r="B44" s="72"/>
+      <c r="C44" s="81"/>
       <c r="D44" s="6" t="s">
         <v>5</v>
       </c>
@@ -5494,10 +5501,10 @@
       <c r="CF44" s="3"/>
     </row>
     <row r="45" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B45" s="60">
+      <c r="B45" s="62">
         <v>16</v>
       </c>
-      <c r="C45" s="61" t="s">
+      <c r="C45" s="77" t="s">
         <v>33</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -5543,14 +5550,14 @@
       <c r="AP45" s="1"/>
       <c r="AQ45" s="1"/>
       <c r="AR45" s="3"/>
-      <c r="AS45" s="93"/>
-      <c r="AT45" s="92"/>
-      <c r="AU45" s="71"/>
-      <c r="AV45" s="71"/>
-      <c r="AW45" s="71"/>
-      <c r="AX45" s="71"/>
-      <c r="AY45" s="71"/>
-      <c r="AZ45" s="72"/>
+      <c r="AS45" s="4"/>
+      <c r="AT45" s="1"/>
+      <c r="AU45" s="41"/>
+      <c r="AV45" s="41"/>
+      <c r="AW45" s="41"/>
+      <c r="AX45" s="41"/>
+      <c r="AY45" s="41"/>
+      <c r="AZ45" s="42"/>
       <c r="BA45" s="4"/>
       <c r="BB45" s="1"/>
       <c r="BC45" s="1"/>
@@ -5585,8 +5592,8 @@
       <c r="CF45" s="3"/>
     </row>
     <row r="46" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B46" s="52"/>
-      <c r="C46" s="63"/>
+      <c r="B46" s="72"/>
+      <c r="C46" s="81"/>
       <c r="D46" s="6" t="s">
         <v>5</v>
       </c>
@@ -5672,7 +5679,7 @@
       <c r="CF46" s="3"/>
     </row>
     <row r="47" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B47" s="60">
+      <c r="B47" s="62">
         <v>17</v>
       </c>
       <c r="C47" s="73" t="s">
@@ -5729,19 +5736,19 @@
       <c r="AX47" s="1"/>
       <c r="AY47" s="1"/>
       <c r="AZ47" s="3"/>
-      <c r="BA47" s="70"/>
-      <c r="BB47" s="71"/>
-      <c r="BC47" s="71"/>
-      <c r="BD47" s="71"/>
-      <c r="BE47" s="71"/>
-      <c r="BF47" s="71"/>
-      <c r="BG47" s="71"/>
-      <c r="BH47" s="75"/>
-      <c r="BI47" s="70"/>
-      <c r="BJ47" s="71"/>
-      <c r="BK47" s="71"/>
-      <c r="BL47" s="71"/>
-      <c r="BM47" s="71"/>
+      <c r="BA47" s="40"/>
+      <c r="BB47" s="41"/>
+      <c r="BC47" s="41"/>
+      <c r="BD47" s="41"/>
+      <c r="BE47" s="41"/>
+      <c r="BF47" s="41"/>
+      <c r="BG47" s="41"/>
+      <c r="BH47" s="43"/>
+      <c r="BI47" s="40"/>
+      <c r="BJ47" s="41"/>
+      <c r="BK47" s="41"/>
+      <c r="BL47" s="41"/>
+      <c r="BM47" s="41"/>
       <c r="BN47" s="1"/>
       <c r="BO47" s="1"/>
       <c r="BP47" s="3"/>
@@ -5760,11 +5767,11 @@
       <c r="CC47" s="1"/>
       <c r="CD47" s="1"/>
       <c r="CE47" s="1"/>
-      <c r="CF47" s="76"/>
+      <c r="CF47" s="44"/>
     </row>
     <row r="48" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B48" s="52"/>
-      <c r="C48" s="55"/>
+      <c r="B48" s="72"/>
+      <c r="C48" s="76"/>
       <c r="D48" s="6" t="s">
         <v>5</v>
       </c>
@@ -5850,10 +5857,10 @@
       <c r="CF48" s="3"/>
     </row>
     <row r="49" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B49" s="60">
+      <c r="B49" s="62">
         <v>18</v>
       </c>
-      <c r="C49" s="61" t="s">
+      <c r="C49" s="77" t="s">
         <v>35</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -5920,8 +5927,8 @@
       <c r="BK49" s="1"/>
       <c r="BL49" s="1"/>
       <c r="BM49" s="1"/>
-      <c r="BN49" s="71"/>
-      <c r="BO49" s="71"/>
+      <c r="BN49" s="41"/>
+      <c r="BO49" s="41"/>
       <c r="BP49" s="3"/>
       <c r="BQ49" s="31"/>
       <c r="BR49" s="1"/>
@@ -5941,8 +5948,8 @@
       <c r="CF49" s="3"/>
     </row>
     <row r="50" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="53"/>
-      <c r="C50" s="62"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="78"/>
       <c r="D50" s="6" t="s">
         <v>5</v>
       </c>
@@ -6028,10 +6035,10 @@
       <c r="CF50" s="3"/>
     </row>
     <row r="51" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B51" s="47" t="s">
+      <c r="B51" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="48"/>
+      <c r="C51" s="65"/>
       <c r="D51" s="8" t="s">
         <v>4</v>
       </c>
@@ -6097,7 +6104,7 @@
       <c r="BL51" s="15"/>
       <c r="BM51" s="15"/>
       <c r="BN51" s="15"/>
-      <c r="BO51" s="71"/>
+      <c r="BO51" s="41"/>
       <c r="BP51" s="20"/>
       <c r="BQ51" s="22"/>
       <c r="BR51" s="15"/>
@@ -6117,8 +6124,8 @@
       <c r="CF51" s="20"/>
     </row>
     <row r="52" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="49"/>
-      <c r="C52" s="50"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="67"/>
       <c r="D52" s="9" t="s">
         <v>5</v>
       </c>
@@ -6291,10 +6298,10 @@
       <c r="CF53" s="21"/>
     </row>
     <row r="54" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B54" s="51">
+      <c r="B54" s="71">
         <v>19</v>
       </c>
-      <c r="C54" s="54" t="s">
+      <c r="C54" s="75" t="s">
         <v>36</v>
       </c>
       <c r="D54" s="5" t="s">
@@ -6363,7 +6370,7 @@
       <c r="BM54" s="1"/>
       <c r="BN54" s="1"/>
       <c r="BO54" s="1"/>
-      <c r="BP54" s="72"/>
+      <c r="BP54" s="42"/>
       <c r="BQ54" s="31"/>
       <c r="BR54" s="1"/>
       <c r="BS54" s="1"/>
@@ -6382,8 +6389,8 @@
       <c r="CF54" s="3"/>
     </row>
     <row r="55" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B55" s="52"/>
-      <c r="C55" s="55"/>
+      <c r="B55" s="72"/>
+      <c r="C55" s="76"/>
       <c r="D55" s="6" t="s">
         <v>5</v>
       </c>
@@ -6469,10 +6476,10 @@
       <c r="CF55" s="3"/>
     </row>
     <row r="56" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B56" s="60">
+      <c r="B56" s="62">
         <v>20</v>
       </c>
-      <c r="C56" s="60" t="s">
+      <c r="C56" s="62" t="s">
         <v>37</v>
       </c>
       <c r="D56" s="6" t="s">
@@ -6542,8 +6549,8 @@
       <c r="BN56" s="1"/>
       <c r="BO56" s="1"/>
       <c r="BP56" s="3"/>
-      <c r="BQ56" s="77"/>
-      <c r="BR56" s="71"/>
+      <c r="BQ56" s="45"/>
+      <c r="BR56" s="41"/>
       <c r="BS56" s="1"/>
       <c r="BT56" s="1"/>
       <c r="BU56" s="1"/>
@@ -6560,8 +6567,8 @@
       <c r="CF56" s="3"/>
     </row>
     <row r="57" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B57" s="52"/>
-      <c r="C57" s="52"/>
+      <c r="B57" s="72"/>
+      <c r="C57" s="72"/>
       <c r="D57" s="6" t="s">
         <v>5</v>
       </c>
@@ -6647,7 +6654,7 @@
       <c r="CF57" s="3"/>
     </row>
     <row r="58" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B58" s="60">
+      <c r="B58" s="62">
         <v>21</v>
       </c>
       <c r="C58" s="73" t="s">
@@ -6722,8 +6729,8 @@
       <c r="BP58" s="3"/>
       <c r="BQ58" s="31"/>
       <c r="BR58" s="1"/>
-      <c r="BS58" s="71"/>
-      <c r="BT58" s="71"/>
+      <c r="BS58" s="41"/>
+      <c r="BT58" s="41"/>
       <c r="BU58" s="1"/>
       <c r="BV58" s="1"/>
       <c r="BW58" s="1"/>
@@ -6738,8 +6745,8 @@
       <c r="CF58" s="3"/>
     </row>
     <row r="59" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B59" s="52"/>
-      <c r="C59" s="55"/>
+      <c r="B59" s="72"/>
+      <c r="C59" s="76"/>
       <c r="D59" s="6" t="s">
         <v>5</v>
       </c>
@@ -6825,7 +6832,7 @@
       <c r="CF59" s="3"/>
     </row>
     <row r="60" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B60" s="60">
+      <c r="B60" s="62">
         <v>22</v>
       </c>
       <c r="C60" s="73" t="s">
@@ -6902,8 +6909,8 @@
       <c r="BR60" s="1"/>
       <c r="BS60" s="1"/>
       <c r="BT60" s="1"/>
-      <c r="BU60" s="71"/>
-      <c r="BV60" s="71"/>
+      <c r="BU60" s="41"/>
+      <c r="BV60" s="41"/>
       <c r="BW60" s="1"/>
       <c r="BX60" s="3"/>
       <c r="BY60" s="4"/>
@@ -6916,8 +6923,8 @@
       <c r="CF60" s="3"/>
     </row>
     <row r="61" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="53"/>
-      <c r="C61" s="78"/>
+      <c r="B61" s="63"/>
+      <c r="C61" s="74"/>
       <c r="D61" s="7" t="s">
         <v>5</v>
       </c>
@@ -7003,10 +7010,10 @@
       <c r="CF61" s="3"/>
     </row>
     <row r="62" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B62" s="47" t="s">
+      <c r="B62" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="48"/>
+      <c r="C62" s="65"/>
       <c r="D62" s="8" t="s">
         <v>4</v>
       </c>
@@ -7079,7 +7086,7 @@
       <c r="BS62" s="15"/>
       <c r="BT62" s="15"/>
       <c r="BU62" s="15"/>
-      <c r="BV62" s="71"/>
+      <c r="BV62" s="41"/>
       <c r="BW62" s="15"/>
       <c r="BX62" s="20"/>
       <c r="BY62" s="18"/>
@@ -7092,8 +7099,8 @@
       <c r="CF62" s="20"/>
     </row>
     <row r="63" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="49"/>
-      <c r="C63" s="50"/>
+      <c r="B63" s="66"/>
+      <c r="C63" s="67"/>
       <c r="D63" s="9" t="s">
         <v>5</v>
       </c>
@@ -7266,10 +7273,10 @@
       <c r="CF64" s="21"/>
     </row>
     <row r="65" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B65" s="51">
+      <c r="B65" s="71">
         <v>23</v>
       </c>
-      <c r="C65" s="54" t="s">
+      <c r="C65" s="75" t="s">
         <v>40</v>
       </c>
       <c r="D65" s="5" t="s">
@@ -7345,20 +7352,20 @@
       <c r="BT65" s="1"/>
       <c r="BU65" s="1"/>
       <c r="BV65" s="1"/>
-      <c r="BW65" s="71"/>
-      <c r="BX65" s="72"/>
-      <c r="BY65" s="70"/>
+      <c r="BW65" s="41"/>
+      <c r="BX65" s="42"/>
+      <c r="BY65" s="40"/>
       <c r="BZ65" s="1"/>
       <c r="CA65" s="1"/>
       <c r="CB65" s="1"/>
       <c r="CC65" s="1"/>
       <c r="CD65" s="1"/>
       <c r="CE65" s="1"/>
-      <c r="CF65" s="79"/>
+      <c r="CF65" s="46"/>
     </row>
     <row r="66" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B66" s="52"/>
-      <c r="C66" s="55"/>
+      <c r="B66" s="72"/>
+      <c r="C66" s="76"/>
       <c r="D66" s="6" t="s">
         <v>5</v>
       </c>
@@ -7444,10 +7451,10 @@
       <c r="CF66" s="3"/>
     </row>
     <row r="67" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B67" s="60">
+      <c r="B67" s="62">
         <v>24</v>
       </c>
-      <c r="C67" s="60" t="s">
+      <c r="C67" s="62" t="s">
         <v>41</v>
       </c>
       <c r="D67" s="6" t="s">
@@ -7526,8 +7533,8 @@
       <c r="BW67" s="1"/>
       <c r="BX67" s="3"/>
       <c r="BY67" s="4"/>
-      <c r="BZ67" s="71"/>
-      <c r="CA67" s="71"/>
+      <c r="BZ67" s="41"/>
+      <c r="CA67" s="41"/>
       <c r="CB67" s="1"/>
       <c r="CC67" s="1"/>
       <c r="CD67" s="1"/>
@@ -7535,8 +7542,8 @@
       <c r="CF67" s="3"/>
     </row>
     <row r="68" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B68" s="52"/>
-      <c r="C68" s="52"/>
+      <c r="B68" s="72"/>
+      <c r="C68" s="72"/>
       <c r="D68" s="6" t="s">
         <v>5</v>
       </c>
@@ -7622,10 +7629,10 @@
       <c r="CF68" s="3"/>
     </row>
     <row r="69" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B69" s="60">
+      <c r="B69" s="62">
         <v>25</v>
       </c>
-      <c r="C69" s="60" t="s">
+      <c r="C69" s="62" t="s">
         <v>42</v>
       </c>
       <c r="D69" s="6" t="s">
@@ -7706,15 +7713,15 @@
       <c r="BY69" s="4"/>
       <c r="BZ69" s="1"/>
       <c r="CA69" s="1"/>
-      <c r="CB69" s="71"/>
-      <c r="CC69" s="71"/>
+      <c r="CB69" s="41"/>
+      <c r="CC69" s="41"/>
       <c r="CD69" s="1"/>
       <c r="CE69" s="1"/>
       <c r="CF69" s="3"/>
     </row>
     <row r="70" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B70" s="52"/>
-      <c r="C70" s="52"/>
+      <c r="B70" s="72"/>
+      <c r="C70" s="72"/>
       <c r="D70" s="6" t="s">
         <v>5</v>
       </c>
@@ -7800,10 +7807,10 @@
       <c r="CF70" s="3"/>
     </row>
     <row r="71" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B71" s="60">
+      <c r="B71" s="62">
         <v>26</v>
       </c>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="62" t="s">
         <v>43</v>
       </c>
       <c r="D71" s="6" t="s">
@@ -7886,13 +7893,13 @@
       <c r="CA71" s="1"/>
       <c r="CB71" s="1"/>
       <c r="CC71" s="1"/>
-      <c r="CD71" s="71"/>
-      <c r="CE71" s="71"/>
+      <c r="CD71" s="41"/>
+      <c r="CE71" s="41"/>
       <c r="CF71" s="3"/>
     </row>
     <row r="72" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="53"/>
-      <c r="C72" s="53"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="63"/>
       <c r="D72" s="7" t="s">
         <v>5</v>
       </c>
@@ -7978,10 +7985,10 @@
       <c r="CF72" s="3"/>
     </row>
     <row r="73" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B73" s="47" t="s">
+      <c r="B73" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C73" s="48"/>
+      <c r="C73" s="65"/>
       <c r="D73" s="8" t="s">
         <v>4</v>
       </c>
@@ -8063,12 +8070,12 @@
       <c r="CB73" s="15"/>
       <c r="CC73" s="15"/>
       <c r="CD73" s="15"/>
-      <c r="CE73" s="71"/>
+      <c r="CE73" s="41"/>
       <c r="CF73" s="20"/>
     </row>
     <row r="74" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="49"/>
-      <c r="C74" s="50"/>
+      <c r="B74" s="66"/>
+      <c r="C74" s="67"/>
       <c r="D74" s="9" t="s">
         <v>5</v>
       </c>
@@ -8241,10 +8248,10 @@
       <c r="CF75" s="21"/>
     </row>
     <row r="76" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B76" s="51">
+      <c r="B76" s="71">
         <v>27</v>
       </c>
-      <c r="C76" s="51" t="s">
+      <c r="C76" s="71" t="s">
         <v>44</v>
       </c>
       <c r="D76" s="5" t="s">
@@ -8255,85 +8262,85 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
-      <c r="J76" s="71"/>
-      <c r="K76" s="71"/>
-      <c r="L76" s="72"/>
+      <c r="J76" s="41"/>
+      <c r="K76" s="41"/>
+      <c r="L76" s="42"/>
       <c r="M76" s="4"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
-      <c r="R76" s="71"/>
-      <c r="S76" s="71"/>
-      <c r="T76" s="72"/>
+      <c r="R76" s="41"/>
+      <c r="S76" s="41"/>
+      <c r="T76" s="42"/>
       <c r="U76" s="4"/>
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
       <c r="X76" s="1"/>
       <c r="Y76" s="1"/>
-      <c r="Z76" s="71"/>
-      <c r="AA76" s="71"/>
-      <c r="AB76" s="72"/>
+      <c r="Z76" s="41"/>
+      <c r="AA76" s="41"/>
+      <c r="AB76" s="42"/>
       <c r="AC76" s="4"/>
       <c r="AD76" s="1"/>
       <c r="AE76" s="1"/>
       <c r="AF76" s="1"/>
       <c r="AG76" s="1"/>
-      <c r="AH76" s="71"/>
-      <c r="AI76" s="71"/>
-      <c r="AJ76" s="72"/>
+      <c r="AH76" s="41"/>
+      <c r="AI76" s="41"/>
+      <c r="AJ76" s="42"/>
       <c r="AK76" s="4"/>
       <c r="AL76" s="1"/>
       <c r="AM76" s="1"/>
       <c r="AN76" s="1"/>
       <c r="AO76" s="1"/>
-      <c r="AP76" s="71"/>
-      <c r="AQ76" s="71"/>
-      <c r="AR76" s="72"/>
+      <c r="AP76" s="41"/>
+      <c r="AQ76" s="41"/>
+      <c r="AR76" s="42"/>
       <c r="AS76" s="4"/>
       <c r="AT76" s="1"/>
       <c r="AU76" s="1"/>
       <c r="AV76" s="1"/>
       <c r="AW76" s="1"/>
-      <c r="AX76" s="71"/>
-      <c r="AY76" s="71"/>
-      <c r="AZ76" s="72"/>
+      <c r="AX76" s="41"/>
+      <c r="AY76" s="41"/>
+      <c r="AZ76" s="42"/>
       <c r="BA76" s="4"/>
       <c r="BB76" s="1"/>
       <c r="BC76" s="1"/>
       <c r="BD76" s="1"/>
       <c r="BE76" s="1"/>
-      <c r="BF76" s="71"/>
-      <c r="BG76" s="71"/>
-      <c r="BH76" s="75"/>
+      <c r="BF76" s="41"/>
+      <c r="BG76" s="41"/>
+      <c r="BH76" s="43"/>
       <c r="BI76" s="4"/>
       <c r="BJ76" s="1"/>
       <c r="BK76" s="1"/>
       <c r="BL76" s="1"/>
       <c r="BM76" s="1"/>
-      <c r="BN76" s="71"/>
-      <c r="BO76" s="71"/>
-      <c r="BP76" s="72"/>
+      <c r="BN76" s="41"/>
+      <c r="BO76" s="41"/>
+      <c r="BP76" s="42"/>
       <c r="BQ76" s="31"/>
       <c r="BR76" s="1"/>
       <c r="BS76" s="1"/>
       <c r="BT76" s="1"/>
       <c r="BU76" s="1"/>
-      <c r="BV76" s="71"/>
-      <c r="BW76" s="71"/>
-      <c r="BX76" s="72"/>
+      <c r="BV76" s="41"/>
+      <c r="BW76" s="41"/>
+      <c r="BX76" s="42"/>
       <c r="BY76" s="4"/>
       <c r="BZ76" s="1"/>
       <c r="CA76" s="1"/>
       <c r="CB76" s="1"/>
       <c r="CC76" s="1"/>
-      <c r="CD76" s="71"/>
-      <c r="CE76" s="71"/>
-      <c r="CF76" s="72"/>
+      <c r="CD76" s="41"/>
+      <c r="CE76" s="41"/>
+      <c r="CF76" s="42"/>
     </row>
     <row r="77" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="53"/>
-      <c r="C77" s="52"/>
+      <c r="B77" s="63"/>
+      <c r="C77" s="72"/>
       <c r="D77" s="6" t="s">
         <v>5</v>
       </c>
@@ -8342,17 +8349,17 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="3"/>
+      <c r="J77" s="54"/>
+      <c r="K77" s="54"/>
+      <c r="L77" s="59"/>
       <c r="M77" s="4"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-      <c r="S77" s="1"/>
-      <c r="T77" s="3"/>
+      <c r="R77" s="54"/>
+      <c r="S77" s="54"/>
+      <c r="T77" s="59"/>
       <c r="U77" s="4"/>
       <c r="V77" s="1"/>
       <c r="W77" s="1"/>
@@ -8419,10 +8426,10 @@
       <c r="CF77" s="3"/>
     </row>
     <row r="78" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B78" s="51">
+      <c r="B78" s="71">
         <v>28</v>
       </c>
-      <c r="C78" s="60" t="s">
+      <c r="C78" s="62" t="s">
         <v>45</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -8441,7 +8448,7 @@
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
-      <c r="R78" s="71"/>
+      <c r="R78" s="41"/>
       <c r="S78" s="1"/>
       <c r="T78" s="3"/>
       <c r="U78" s="4"/>
@@ -8510,8 +8517,8 @@
       <c r="CF78" s="3"/>
     </row>
     <row r="79" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B79" s="52"/>
-      <c r="C79" s="52"/>
+      <c r="B79" s="72"/>
+      <c r="C79" s="72"/>
       <c r="D79" s="6" t="s">
         <v>5</v>
       </c>
@@ -8528,7 +8535,7 @@
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
-      <c r="R79" s="1"/>
+      <c r="R79" s="54"/>
       <c r="S79" s="1"/>
       <c r="T79" s="3"/>
       <c r="U79" s="4"/>
@@ -8597,10 +8604,10 @@
       <c r="CF79" s="3"/>
     </row>
     <row r="80" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B80" s="60">
+      <c r="B80" s="62">
         <v>29</v>
       </c>
-      <c r="C80" s="60" t="s">
+      <c r="C80" s="62" t="s">
         <v>46</v>
       </c>
       <c r="D80" s="6" t="s">
@@ -8613,7 +8620,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
-      <c r="L80" s="72"/>
+      <c r="L80" s="42"/>
       <c r="M80" s="4"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
@@ -8621,7 +8628,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
-      <c r="T80" s="72"/>
+      <c r="T80" s="42"/>
       <c r="U80" s="4"/>
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
@@ -8629,7 +8636,7 @@
       <c r="Y80" s="1"/>
       <c r="Z80" s="1"/>
       <c r="AA80" s="1"/>
-      <c r="AB80" s="72"/>
+      <c r="AB80" s="42"/>
       <c r="AC80" s="4"/>
       <c r="AD80" s="1"/>
       <c r="AE80" s="1"/>
@@ -8637,7 +8644,7 @@
       <c r="AG80" s="1"/>
       <c r="AH80" s="1"/>
       <c r="AI80" s="1"/>
-      <c r="AJ80" s="72"/>
+      <c r="AJ80" s="42"/>
       <c r="AK80" s="4"/>
       <c r="AL80" s="1"/>
       <c r="AM80" s="1"/>
@@ -8645,7 +8652,7 @@
       <c r="AO80" s="1"/>
       <c r="AP80" s="1"/>
       <c r="AQ80" s="1"/>
-      <c r="AR80" s="72"/>
+      <c r="AR80" s="42"/>
       <c r="AS80" s="4"/>
       <c r="AT80" s="1"/>
       <c r="AU80" s="1"/>
@@ -8653,7 +8660,7 @@
       <c r="AW80" s="1"/>
       <c r="AX80" s="1"/>
       <c r="AY80" s="1"/>
-      <c r="AZ80" s="72"/>
+      <c r="AZ80" s="42"/>
       <c r="BA80" s="4"/>
       <c r="BB80" s="1"/>
       <c r="BC80" s="1"/>
@@ -8661,7 +8668,7 @@
       <c r="BE80" s="1"/>
       <c r="BF80" s="1"/>
       <c r="BG80" s="1"/>
-      <c r="BH80" s="75"/>
+      <c r="BH80" s="43"/>
       <c r="BI80" s="4"/>
       <c r="BJ80" s="1"/>
       <c r="BK80" s="1"/>
@@ -8669,7 +8676,7 @@
       <c r="BM80" s="1"/>
       <c r="BN80" s="1"/>
       <c r="BO80" s="1"/>
-      <c r="BP80" s="72"/>
+      <c r="BP80" s="42"/>
       <c r="BQ80" s="31"/>
       <c r="BR80" s="1"/>
       <c r="BS80" s="1"/>
@@ -8677,7 +8684,7 @@
       <c r="BU80" s="1"/>
       <c r="BV80" s="1"/>
       <c r="BW80" s="1"/>
-      <c r="BX80" s="72"/>
+      <c r="BX80" s="42"/>
       <c r="BY80" s="4"/>
       <c r="BZ80" s="1"/>
       <c r="CA80" s="1"/>
@@ -8685,100 +8692,100 @@
       <c r="CC80" s="1"/>
       <c r="CD80" s="1"/>
       <c r="CE80" s="1"/>
-      <c r="CF80" s="72"/>
+      <c r="CF80" s="42"/>
     </row>
     <row r="81" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="53"/>
-      <c r="C81" s="53"/>
-      <c r="D81" s="80" t="s">
+      <c r="B81" s="63"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="E81" s="81"/>
-      <c r="F81" s="82"/>
-      <c r="G81" s="82"/>
-      <c r="H81" s="82"/>
-      <c r="I81" s="82"/>
-      <c r="J81" s="82"/>
-      <c r="K81" s="82"/>
-      <c r="L81" s="83"/>
-      <c r="M81" s="81"/>
-      <c r="N81" s="82"/>
-      <c r="O81" s="82"/>
-      <c r="P81" s="82"/>
-      <c r="Q81" s="82"/>
-      <c r="R81" s="82"/>
-      <c r="S81" s="82"/>
-      <c r="T81" s="83"/>
-      <c r="U81" s="81"/>
-      <c r="V81" s="82"/>
-      <c r="W81" s="82"/>
-      <c r="X81" s="82"/>
-      <c r="Y81" s="82"/>
-      <c r="Z81" s="82"/>
-      <c r="AA81" s="82"/>
-      <c r="AB81" s="83"/>
-      <c r="AC81" s="81"/>
-      <c r="AD81" s="82"/>
-      <c r="AE81" s="82"/>
-      <c r="AF81" s="82"/>
-      <c r="AG81" s="82"/>
-      <c r="AH81" s="82"/>
-      <c r="AI81" s="82"/>
-      <c r="AJ81" s="83"/>
-      <c r="AK81" s="81"/>
-      <c r="AL81" s="82"/>
-      <c r="AM81" s="82"/>
-      <c r="AN81" s="82"/>
-      <c r="AO81" s="82"/>
-      <c r="AP81" s="82"/>
-      <c r="AQ81" s="82"/>
-      <c r="AR81" s="83"/>
-      <c r="AS81" s="81"/>
-      <c r="AT81" s="82"/>
-      <c r="AU81" s="82"/>
-      <c r="AV81" s="82"/>
-      <c r="AW81" s="82"/>
-      <c r="AX81" s="82"/>
-      <c r="AY81" s="82"/>
-      <c r="AZ81" s="83"/>
-      <c r="BA81" s="81"/>
-      <c r="BB81" s="82"/>
-      <c r="BC81" s="82"/>
-      <c r="BD81" s="82"/>
-      <c r="BE81" s="82"/>
-      <c r="BF81" s="82"/>
-      <c r="BG81" s="82"/>
-      <c r="BH81" s="84"/>
-      <c r="BI81" s="81"/>
-      <c r="BJ81" s="82"/>
-      <c r="BK81" s="82"/>
-      <c r="BL81" s="82"/>
-      <c r="BM81" s="82"/>
-      <c r="BN81" s="82"/>
-      <c r="BO81" s="82"/>
-      <c r="BP81" s="83"/>
-      <c r="BQ81" s="85"/>
-      <c r="BR81" s="82"/>
-      <c r="BS81" s="82"/>
-      <c r="BT81" s="82"/>
-      <c r="BU81" s="82"/>
-      <c r="BV81" s="82"/>
-      <c r="BW81" s="82"/>
-      <c r="BX81" s="83"/>
-      <c r="BY81" s="81"/>
-      <c r="BZ81" s="82"/>
-      <c r="CA81" s="82"/>
-      <c r="CB81" s="82"/>
-      <c r="CC81" s="82"/>
-      <c r="CD81" s="82"/>
-      <c r="CE81" s="82"/>
-      <c r="CF81" s="83"/>
+      <c r="E81" s="48"/>
+      <c r="F81" s="49"/>
+      <c r="G81" s="49"/>
+      <c r="H81" s="49"/>
+      <c r="I81" s="49"/>
+      <c r="J81" s="49"/>
+      <c r="K81" s="49"/>
+      <c r="L81" s="99"/>
+      <c r="M81" s="48"/>
+      <c r="N81" s="49"/>
+      <c r="O81" s="49"/>
+      <c r="P81" s="49"/>
+      <c r="Q81" s="49"/>
+      <c r="R81" s="49"/>
+      <c r="S81" s="49"/>
+      <c r="T81" s="99"/>
+      <c r="U81" s="48"/>
+      <c r="V81" s="49"/>
+      <c r="W81" s="49"/>
+      <c r="X81" s="49"/>
+      <c r="Y81" s="49"/>
+      <c r="Z81" s="49"/>
+      <c r="AA81" s="49"/>
+      <c r="AB81" s="50"/>
+      <c r="AC81" s="48"/>
+      <c r="AD81" s="49"/>
+      <c r="AE81" s="49"/>
+      <c r="AF81" s="49"/>
+      <c r="AG81" s="49"/>
+      <c r="AH81" s="49"/>
+      <c r="AI81" s="49"/>
+      <c r="AJ81" s="50"/>
+      <c r="AK81" s="48"/>
+      <c r="AL81" s="49"/>
+      <c r="AM81" s="49"/>
+      <c r="AN81" s="49"/>
+      <c r="AO81" s="49"/>
+      <c r="AP81" s="49"/>
+      <c r="AQ81" s="49"/>
+      <c r="AR81" s="50"/>
+      <c r="AS81" s="48"/>
+      <c r="AT81" s="49"/>
+      <c r="AU81" s="49"/>
+      <c r="AV81" s="49"/>
+      <c r="AW81" s="49"/>
+      <c r="AX81" s="49"/>
+      <c r="AY81" s="49"/>
+      <c r="AZ81" s="50"/>
+      <c r="BA81" s="48"/>
+      <c r="BB81" s="49"/>
+      <c r="BC81" s="49"/>
+      <c r="BD81" s="49"/>
+      <c r="BE81" s="49"/>
+      <c r="BF81" s="49"/>
+      <c r="BG81" s="49"/>
+      <c r="BH81" s="51"/>
+      <c r="BI81" s="48"/>
+      <c r="BJ81" s="49"/>
+      <c r="BK81" s="49"/>
+      <c r="BL81" s="49"/>
+      <c r="BM81" s="49"/>
+      <c r="BN81" s="49"/>
+      <c r="BO81" s="49"/>
+      <c r="BP81" s="50"/>
+      <c r="BQ81" s="52"/>
+      <c r="BR81" s="49"/>
+      <c r="BS81" s="49"/>
+      <c r="BT81" s="49"/>
+      <c r="BU81" s="49"/>
+      <c r="BV81" s="49"/>
+      <c r="BW81" s="49"/>
+      <c r="BX81" s="50"/>
+      <c r="BY81" s="48"/>
+      <c r="BZ81" s="49"/>
+      <c r="CA81" s="49"/>
+      <c r="CB81" s="49"/>
+      <c r="CC81" s="49"/>
+      <c r="CD81" s="49"/>
+      <c r="CE81" s="49"/>
+      <c r="CF81" s="50"/>
     </row>
     <row r="82" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B82" s="47" t="s">
+      <c r="B82" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="C82" s="48"/>
+      <c r="C82" s="65"/>
       <c r="D82" s="8" t="s">
         <v>4</v>
       </c>
@@ -8861,11 +8868,11 @@
       <c r="CC82" s="15"/>
       <c r="CD82" s="15"/>
       <c r="CE82" s="15"/>
-      <c r="CF82" s="72"/>
+      <c r="CF82" s="42"/>
     </row>
     <row r="83" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="49"/>
-      <c r="C83" s="50"/>
+      <c r="B83" s="66"/>
+      <c r="C83" s="67"/>
       <c r="D83" s="9" t="s">
         <v>5</v>
       </c>
@@ -8951,85 +8958,47 @@
       <c r="CF83" s="28"/>
     </row>
     <row r="84" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="44" t="s">
+      <c r="B84" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C84" s="45"/>
-      <c r="D84" s="46"/>
-      <c r="E84" s="88"/>
-      <c r="F84" s="89" t="s">
+      <c r="C84" s="69"/>
+      <c r="D84" s="70"/>
+      <c r="E84" s="55"/>
+      <c r="F84" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G84" s="43"/>
-      <c r="H84" s="90"/>
-      <c r="I84" s="89" t="s">
+      <c r="G84" s="61"/>
+      <c r="H84" s="56"/>
+      <c r="I84" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="J84" s="43"/>
-      <c r="K84" s="91"/>
-      <c r="L84" s="89" t="s">
+      <c r="J84" s="61"/>
+      <c r="K84" s="57"/>
+      <c r="L84" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="M84" s="43"/>
+      <c r="M84" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="B82:C83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="B73:C74"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="B51:C52"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="BY2:CF2"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
     <mergeCell ref="BQ2:BX2"/>
     <mergeCell ref="E2:L2"/>
     <mergeCell ref="M2:T2"/>
@@ -9039,24 +9008,62 @@
     <mergeCell ref="AS2:AZ2"/>
     <mergeCell ref="BA2:BH2"/>
     <mergeCell ref="BI2:BP2"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="BY2:CF2"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="B51:C52"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="B73:C74"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="B82:C83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="F84:G84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="38" fitToWidth="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 1.5 IPA Tag 3
- Planung des Testkonzepts abgeschlossen. Planen-Phase abgeschlossen.
- Approval-Meeting und Protokollierung abgeschlossen, sowie resultierende Änderungen an der Testumgebung und der Grundschutzstufen notiert.
- Festlegung Externer Hilfestellung dokumentiert. Abschluss der Entscheiden-Phase
- Nummern der Dokumente angepasst
</commit_message>
<xml_diff>
--- a/02_Zeitplanung_Nideröst.xlsx
+++ b/02_Zeitplanung_Nideröst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\IPA_Nideröst_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F716FA-A914-4AC3-9B6E-18291041CA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF9DA6C-C870-486D-836A-0F74148A05A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" xr2:uid="{8796DB52-94B7-4869-AF39-88ED6CB3CCF9}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -825,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -902,6 +903,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -977,18 +980,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,15 +998,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1342,8 +1342,8 @@
   </sheetPr>
   <dimension ref="B1:CF84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="U70" sqref="U70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,120 +1355,120 @@
   <sheetData>
     <row r="1" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="87">
+      <c r="E2" s="95">
         <v>45376</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="95">
         <v>45377</v>
       </c>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="87">
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="94"/>
+      <c r="U2" s="95">
         <v>45378</v>
       </c>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85"/>
-      <c r="X2" s="85"/>
-      <c r="Y2" s="85"/>
-      <c r="Z2" s="85"/>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="86"/>
-      <c r="AC2" s="87">
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="93"/>
+      <c r="Y2" s="93"/>
+      <c r="Z2" s="93"/>
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="94"/>
+      <c r="AC2" s="95">
         <v>45384</v>
       </c>
-      <c r="AD2" s="85"/>
-      <c r="AE2" s="85"/>
-      <c r="AF2" s="85"/>
-      <c r="AG2" s="85"/>
-      <c r="AH2" s="85"/>
-      <c r="AI2" s="85"/>
-      <c r="AJ2" s="86"/>
-      <c r="AK2" s="87">
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="93"/>
+      <c r="AG2" s="93"/>
+      <c r="AH2" s="93"/>
+      <c r="AI2" s="93"/>
+      <c r="AJ2" s="94"/>
+      <c r="AK2" s="95">
         <v>45385</v>
       </c>
-      <c r="AL2" s="85"/>
-      <c r="AM2" s="85"/>
-      <c r="AN2" s="85"/>
-      <c r="AO2" s="85"/>
-      <c r="AP2" s="85"/>
-      <c r="AQ2" s="85"/>
-      <c r="AR2" s="86"/>
-      <c r="AS2" s="87">
+      <c r="AL2" s="93"/>
+      <c r="AM2" s="93"/>
+      <c r="AN2" s="93"/>
+      <c r="AO2" s="93"/>
+      <c r="AP2" s="93"/>
+      <c r="AQ2" s="93"/>
+      <c r="AR2" s="94"/>
+      <c r="AS2" s="95">
         <v>45387</v>
       </c>
-      <c r="AT2" s="85"/>
-      <c r="AU2" s="85"/>
-      <c r="AV2" s="85"/>
-      <c r="AW2" s="85"/>
-      <c r="AX2" s="85"/>
-      <c r="AY2" s="85"/>
-      <c r="AZ2" s="86"/>
-      <c r="BA2" s="87">
+      <c r="AT2" s="93"/>
+      <c r="AU2" s="93"/>
+      <c r="AV2" s="93"/>
+      <c r="AW2" s="93"/>
+      <c r="AX2" s="93"/>
+      <c r="AY2" s="93"/>
+      <c r="AZ2" s="94"/>
+      <c r="BA2" s="95">
         <v>45390</v>
       </c>
-      <c r="BB2" s="85"/>
-      <c r="BC2" s="85"/>
-      <c r="BD2" s="85"/>
-      <c r="BE2" s="85"/>
-      <c r="BF2" s="85"/>
-      <c r="BG2" s="85"/>
-      <c r="BH2" s="85"/>
-      <c r="BI2" s="87">
+      <c r="BB2" s="93"/>
+      <c r="BC2" s="93"/>
+      <c r="BD2" s="93"/>
+      <c r="BE2" s="93"/>
+      <c r="BF2" s="93"/>
+      <c r="BG2" s="93"/>
+      <c r="BH2" s="93"/>
+      <c r="BI2" s="95">
         <v>45391</v>
       </c>
-      <c r="BJ2" s="85"/>
-      <c r="BK2" s="85"/>
-      <c r="BL2" s="85"/>
-      <c r="BM2" s="85"/>
-      <c r="BN2" s="85"/>
-      <c r="BO2" s="85"/>
-      <c r="BP2" s="86"/>
-      <c r="BQ2" s="85">
+      <c r="BJ2" s="93"/>
+      <c r="BK2" s="93"/>
+      <c r="BL2" s="93"/>
+      <c r="BM2" s="93"/>
+      <c r="BN2" s="93"/>
+      <c r="BO2" s="93"/>
+      <c r="BP2" s="94"/>
+      <c r="BQ2" s="93">
         <v>45392</v>
       </c>
-      <c r="BR2" s="85"/>
-      <c r="BS2" s="85"/>
-      <c r="BT2" s="85"/>
-      <c r="BU2" s="85"/>
-      <c r="BV2" s="85"/>
-      <c r="BW2" s="85"/>
-      <c r="BX2" s="86"/>
-      <c r="BY2" s="87">
+      <c r="BR2" s="93"/>
+      <c r="BS2" s="93"/>
+      <c r="BT2" s="93"/>
+      <c r="BU2" s="93"/>
+      <c r="BV2" s="93"/>
+      <c r="BW2" s="93"/>
+      <c r="BX2" s="94"/>
+      <c r="BY2" s="95">
         <v>45394</v>
       </c>
-      <c r="BZ2" s="85"/>
-      <c r="CA2" s="85"/>
-      <c r="CB2" s="85"/>
-      <c r="CC2" s="85"/>
-      <c r="CD2" s="85"/>
-      <c r="CE2" s="85"/>
-      <c r="CF2" s="86"/>
+      <c r="BZ2" s="93"/>
+      <c r="CA2" s="93"/>
+      <c r="CB2" s="93"/>
+      <c r="CC2" s="93"/>
+      <c r="CD2" s="93"/>
+      <c r="CE2" s="93"/>
+      <c r="CF2" s="94"/>
     </row>
     <row r="3" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="93"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="91"/>
       <c r="E3" s="25" t="s">
         <v>2</v>
       </c>
@@ -1711,9 +1711,9 @@
       </c>
     </row>
     <row r="4" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="94"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
@@ -1956,10 +1956,10 @@
       </c>
     </row>
     <row r="5" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="96"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="12"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
@@ -2043,10 +2043,10 @@
       <c r="CF5" s="24"/>
     </row>
     <row r="6" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="71">
+      <c r="B6" s="73">
         <v>1</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="96" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -2134,8 +2134,8 @@
       <c r="CF6" s="3"/>
     </row>
     <row r="7" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="72"/>
-      <c r="C7" s="80"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="82"/>
       <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
@@ -2221,10 +2221,10 @@
       <c r="CF7" s="3"/>
     </row>
     <row r="8" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="62">
+      <c r="B8" s="64">
         <v>2</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="79" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -2312,8 +2312,8 @@
       <c r="CF8" s="3"/>
     </row>
     <row r="9" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="72"/>
-      <c r="C9" s="81"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="6" t="s">
         <v>5</v>
       </c>
@@ -2399,10 +2399,10 @@
       <c r="CF9" s="3"/>
     </row>
     <row r="10" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="62">
+      <c r="B10" s="64">
         <v>3</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="79" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -2490,8 +2490,8 @@
       <c r="CF10" s="3"/>
     </row>
     <row r="11" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="63"/>
-      <c r="C11" s="78"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
@@ -2577,10 +2577,10 @@
       <c r="CF11" s="3"/>
     </row>
     <row r="12" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="8" t="s">
         <v>4</v>
       </c>
@@ -2666,8 +2666,8 @@
       <c r="CF12" s="20"/>
     </row>
     <row r="13" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="9" t="s">
         <v>5</v>
       </c>
@@ -2840,10 +2840,10 @@
       <c r="CF14" s="21"/>
     </row>
     <row r="15" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="71">
+      <c r="B15" s="73">
         <v>4</v>
       </c>
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="96" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -2931,8 +2931,8 @@
       <c r="CF15" s="3"/>
     </row>
     <row r="16" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="72"/>
-      <c r="C16" s="80"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="6" t="s">
         <v>5</v>
       </c>
@@ -3018,10 +3018,10 @@
       <c r="CF16" s="3"/>
     </row>
     <row r="17" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="62">
+      <c r="B17" s="64">
         <v>5</v>
       </c>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="79" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -3109,8 +3109,8 @@
       <c r="CF17" s="3"/>
     </row>
     <row r="18" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="72"/>
-      <c r="C18" s="81"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="83"/>
       <c r="D18" s="6" t="s">
         <v>5</v>
       </c>
@@ -3196,10 +3196,10 @@
       <c r="CF18" s="3"/>
     </row>
     <row r="19" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="62">
+      <c r="B19" s="64">
         <v>6</v>
       </c>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="79" t="s">
         <v>52</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -3287,8 +3287,8 @@
       <c r="CF19" s="3"/>
     </row>
     <row r="20" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="72"/>
-      <c r="C20" s="81"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="83"/>
       <c r="D20" s="6" t="s">
         <v>5</v>
       </c>
@@ -3304,7 +3304,7 @@
       <c r="N20" s="54"/>
       <c r="O20" s="54"/>
       <c r="P20" s="54"/>
-      <c r="Q20" s="98"/>
+      <c r="Q20" s="60"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="3"/>
@@ -3374,10 +3374,10 @@
       <c r="CF20" s="3"/>
     </row>
     <row r="21" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="62">
+      <c r="B21" s="64">
         <v>7</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="75" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -3465,8 +3465,8 @@
       <c r="CF21" s="3"/>
     </row>
     <row r="22" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="72"/>
-      <c r="C22" s="76"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="6" t="s">
         <v>5</v>
       </c>
@@ -3552,10 +3552,10 @@
       <c r="CF22" s="3"/>
     </row>
     <row r="23" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="62">
+      <c r="B23" s="64">
         <v>8</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="81" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -3642,8 +3642,8 @@
       <c r="CF23" s="3"/>
     </row>
     <row r="24" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="63"/>
-      <c r="C24" s="88"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="96"/>
       <c r="D24" s="7" t="s">
         <v>5</v>
       </c>
@@ -3663,11 +3663,11 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="59"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="54"/>
+      <c r="W24" s="54"/>
       <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
+      <c r="Y24" s="54"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="3"/>
@@ -3729,10 +3729,10 @@
       <c r="CF24" s="3"/>
     </row>
     <row r="25" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="65"/>
+      <c r="C25" s="67"/>
       <c r="D25" s="8" t="s">
         <v>4</v>
       </c>
@@ -3818,8 +3818,8 @@
       <c r="CF25" s="20"/>
     </row>
     <row r="26" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="66"/>
-      <c r="C26" s="67"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="9" t="s">
         <v>5</v>
       </c>
@@ -3843,7 +3843,7 @@
       <c r="V26" s="15"/>
       <c r="W26" s="15"/>
       <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
+      <c r="Y26" s="54"/>
       <c r="Z26" s="15"/>
       <c r="AA26" s="15"/>
       <c r="AB26" s="20"/>
@@ -3992,10 +3992,10 @@
       <c r="CF27" s="21"/>
     </row>
     <row r="28" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="82">
+      <c r="B28" s="84">
         <v>9</v>
       </c>
-      <c r="C28" s="77" t="s">
+      <c r="C28" s="79" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -4019,7 +4019,7 @@
       <c r="T28" s="3"/>
       <c r="U28" s="4"/>
       <c r="V28" s="1"/>
-      <c r="W28" s="97"/>
+      <c r="W28" s="1"/>
       <c r="X28" s="41"/>
       <c r="Y28" s="41"/>
       <c r="Z28" s="1"/>
@@ -4083,8 +4083,8 @@
       <c r="CF28" s="3"/>
     </row>
     <row r="29" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="83"/>
-      <c r="C29" s="78"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="80"/>
       <c r="D29" s="7" t="s">
         <v>5</v>
       </c>
@@ -4107,7 +4107,7 @@
       <c r="U29" s="4"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
+      <c r="X29" s="54"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
@@ -4170,10 +4170,10 @@
       <c r="CF29" s="3"/>
     </row>
     <row r="30" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="84">
+      <c r="B30" s="86">
         <v>10</v>
       </c>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="79" t="s">
         <v>47</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -4261,8 +4261,8 @@
       <c r="CF30" s="3"/>
     </row>
     <row r="31" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="72"/>
-      <c r="C31" s="81"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="83"/>
       <c r="D31" s="6" t="s">
         <v>5</v>
       </c>
@@ -4287,7 +4287,7 @@
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
+      <c r="Z31" s="54"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="4"/>
@@ -4348,10 +4348,10 @@
       <c r="CF31" s="3"/>
     </row>
     <row r="32" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="62">
+      <c r="B32" s="64">
         <v>11</v>
       </c>
-      <c r="C32" s="77" t="s">
+      <c r="C32" s="79" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -4439,8 +4439,8 @@
       <c r="CF32" s="3"/>
     </row>
     <row r="33" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="63"/>
-      <c r="C33" s="78"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="80"/>
       <c r="D33" s="7" t="s">
         <v>5</v>
       </c>
@@ -4466,8 +4466,8 @@
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="3"/>
+      <c r="AA33" s="54"/>
+      <c r="AB33" s="59"/>
       <c r="AC33" s="4"/>
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
@@ -4526,10 +4526,10 @@
       <c r="CF33" s="3"/>
     </row>
     <row r="34" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="65"/>
+      <c r="C34" s="67"/>
       <c r="D34" s="8" t="s">
         <v>4</v>
       </c>
@@ -4615,8 +4615,8 @@
       <c r="CF34" s="20"/>
     </row>
     <row r="35" spans="2:84" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="66"/>
-      <c r="C35" s="67"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="69"/>
       <c r="D35" s="9" t="s">
         <v>5</v>
       </c>
@@ -4643,7 +4643,7 @@
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
       <c r="AA35" s="15"/>
-      <c r="AB35" s="20"/>
+      <c r="AB35" s="59"/>
       <c r="AC35" s="18"/>
       <c r="AD35" s="15"/>
       <c r="AE35" s="15"/>
@@ -4789,10 +4789,10 @@
       <c r="CF36" s="21"/>
     </row>
     <row r="37" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="71">
+      <c r="B37" s="73">
         <v>12</v>
       </c>
-      <c r="C37" s="78" t="s">
+      <c r="C37" s="80" t="s">
         <v>50</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -4880,8 +4880,8 @@
       <c r="CF37" s="3"/>
     </row>
     <row r="38" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="72"/>
-      <c r="C38" s="81"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="83"/>
       <c r="D38" s="6" t="s">
         <v>5</v>
       </c>
@@ -4967,10 +4967,10 @@
       <c r="CF38" s="3"/>
     </row>
     <row r="39" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="62">
+      <c r="B39" s="64">
         <v>13</v>
       </c>
-      <c r="C39" s="77" t="s">
+      <c r="C39" s="79" t="s">
         <v>30</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -5058,8 +5058,8 @@
       <c r="CF39" s="3"/>
     </row>
     <row r="40" spans="2:84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="72"/>
-      <c r="C40" s="81"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="83"/>
       <c r="D40" s="6" t="s">
         <v>5</v>
       </c>
@@ -5145,10 +5145,10 @@
       <c r="CF40" s="3"/>
     </row>
     <row r="41" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B41" s="62">
+      <c r="B41" s="64">
         <v>14</v>
       </c>
-      <c r="C41" s="79" t="s">
+      <c r="C41" s="81" t="s">
         <v>31</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -5236,8 +5236,8 @@
       <c r="CF41" s="3"/>
     </row>
     <row r="42" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B42" s="72"/>
-      <c r="C42" s="80"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="82"/>
       <c r="D42" s="6" t="s">
         <v>5</v>
       </c>
@@ -5323,10 +5323,10 @@
       <c r="CF42" s="3"/>
     </row>
     <row r="43" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B43" s="62">
+      <c r="B43" s="64">
         <v>15</v>
       </c>
-      <c r="C43" s="77" t="s">
+      <c r="C43" s="79" t="s">
         <v>32</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -5414,8 +5414,8 @@
       <c r="CF43" s="3"/>
     </row>
     <row r="44" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B44" s="72"/>
-      <c r="C44" s="81"/>
+      <c r="B44" s="74"/>
+      <c r="C44" s="83"/>
       <c r="D44" s="6" t="s">
         <v>5</v>
       </c>
@@ -5501,10 +5501,10 @@
       <c r="CF44" s="3"/>
     </row>
     <row r="45" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B45" s="62">
+      <c r="B45" s="64">
         <v>16</v>
       </c>
-      <c r="C45" s="77" t="s">
+      <c r="C45" s="79" t="s">
         <v>33</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -5592,8 +5592,8 @@
       <c r="CF45" s="3"/>
     </row>
     <row r="46" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B46" s="72"/>
-      <c r="C46" s="81"/>
+      <c r="B46" s="74"/>
+      <c r="C46" s="83"/>
       <c r="D46" s="6" t="s">
         <v>5</v>
       </c>
@@ -5679,10 +5679,10 @@
       <c r="CF46" s="3"/>
     </row>
     <row r="47" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B47" s="62">
+      <c r="B47" s="64">
         <v>17</v>
       </c>
-      <c r="C47" s="73" t="s">
+      <c r="C47" s="75" t="s">
         <v>34</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -5770,8 +5770,8 @@
       <c r="CF47" s="44"/>
     </row>
     <row r="48" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B48" s="72"/>
-      <c r="C48" s="76"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="78"/>
       <c r="D48" s="6" t="s">
         <v>5</v>
       </c>
@@ -5857,10 +5857,10 @@
       <c r="CF48" s="3"/>
     </row>
     <row r="49" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B49" s="62">
+      <c r="B49" s="64">
         <v>18</v>
       </c>
-      <c r="C49" s="77" t="s">
+      <c r="C49" s="79" t="s">
         <v>35</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -5948,8 +5948,8 @@
       <c r="CF49" s="3"/>
     </row>
     <row r="50" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="63"/>
-      <c r="C50" s="78"/>
+      <c r="B50" s="65"/>
+      <c r="C50" s="80"/>
       <c r="D50" s="6" t="s">
         <v>5</v>
       </c>
@@ -6035,10 +6035,10 @@
       <c r="CF50" s="3"/>
     </row>
     <row r="51" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B51" s="64" t="s">
+      <c r="B51" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="65"/>
+      <c r="C51" s="67"/>
       <c r="D51" s="8" t="s">
         <v>4</v>
       </c>
@@ -6124,8 +6124,8 @@
       <c r="CF51" s="20"/>
     </row>
     <row r="52" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="66"/>
-      <c r="C52" s="67"/>
+      <c r="B52" s="68"/>
+      <c r="C52" s="69"/>
       <c r="D52" s="9" t="s">
         <v>5</v>
       </c>
@@ -6298,10 +6298,10 @@
       <c r="CF53" s="21"/>
     </row>
     <row r="54" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B54" s="71">
+      <c r="B54" s="73">
         <v>19</v>
       </c>
-      <c r="C54" s="75" t="s">
+      <c r="C54" s="77" t="s">
         <v>36</v>
       </c>
       <c r="D54" s="5" t="s">
@@ -6389,8 +6389,8 @@
       <c r="CF54" s="3"/>
     </row>
     <row r="55" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B55" s="72"/>
-      <c r="C55" s="76"/>
+      <c r="B55" s="74"/>
+      <c r="C55" s="78"/>
       <c r="D55" s="6" t="s">
         <v>5</v>
       </c>
@@ -6476,10 +6476,10 @@
       <c r="CF55" s="3"/>
     </row>
     <row r="56" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B56" s="62">
+      <c r="B56" s="64">
         <v>20</v>
       </c>
-      <c r="C56" s="62" t="s">
+      <c r="C56" s="64" t="s">
         <v>37</v>
       </c>
       <c r="D56" s="6" t="s">
@@ -6567,8 +6567,8 @@
       <c r="CF56" s="3"/>
     </row>
     <row r="57" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B57" s="72"/>
-      <c r="C57" s="72"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="74"/>
       <c r="D57" s="6" t="s">
         <v>5</v>
       </c>
@@ -6654,10 +6654,10 @@
       <c r="CF57" s="3"/>
     </row>
     <row r="58" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B58" s="62">
+      <c r="B58" s="64">
         <v>21</v>
       </c>
-      <c r="C58" s="73" t="s">
+      <c r="C58" s="75" t="s">
         <v>38</v>
       </c>
       <c r="D58" s="6" t="s">
@@ -6745,8 +6745,8 @@
       <c r="CF58" s="3"/>
     </row>
     <row r="59" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B59" s="72"/>
-      <c r="C59" s="76"/>
+      <c r="B59" s="74"/>
+      <c r="C59" s="78"/>
       <c r="D59" s="6" t="s">
         <v>5</v>
       </c>
@@ -6832,10 +6832,10 @@
       <c r="CF59" s="3"/>
     </row>
     <row r="60" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B60" s="62">
+      <c r="B60" s="64">
         <v>22</v>
       </c>
-      <c r="C60" s="73" t="s">
+      <c r="C60" s="75" t="s">
         <v>39</v>
       </c>
       <c r="D60" s="6" t="s">
@@ -6923,8 +6923,8 @@
       <c r="CF60" s="3"/>
     </row>
     <row r="61" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="63"/>
-      <c r="C61" s="74"/>
+      <c r="B61" s="65"/>
+      <c r="C61" s="76"/>
       <c r="D61" s="7" t="s">
         <v>5</v>
       </c>
@@ -7010,10 +7010,10 @@
       <c r="CF61" s="3"/>
     </row>
     <row r="62" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B62" s="64" t="s">
+      <c r="B62" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="65"/>
+      <c r="C62" s="67"/>
       <c r="D62" s="8" t="s">
         <v>4</v>
       </c>
@@ -7099,8 +7099,8 @@
       <c r="CF62" s="20"/>
     </row>
     <row r="63" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="66"/>
-      <c r="C63" s="67"/>
+      <c r="B63" s="68"/>
+      <c r="C63" s="69"/>
       <c r="D63" s="9" t="s">
         <v>5</v>
       </c>
@@ -7273,10 +7273,10 @@
       <c r="CF64" s="21"/>
     </row>
     <row r="65" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B65" s="71">
+      <c r="B65" s="73">
         <v>23</v>
       </c>
-      <c r="C65" s="75" t="s">
+      <c r="C65" s="77" t="s">
         <v>40</v>
       </c>
       <c r="D65" s="5" t="s">
@@ -7364,8 +7364,8 @@
       <c r="CF65" s="46"/>
     </row>
     <row r="66" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B66" s="72"/>
-      <c r="C66" s="76"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="78"/>
       <c r="D66" s="6" t="s">
         <v>5</v>
       </c>
@@ -7451,10 +7451,10 @@
       <c r="CF66" s="3"/>
     </row>
     <row r="67" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B67" s="62">
+      <c r="B67" s="64">
         <v>24</v>
       </c>
-      <c r="C67" s="62" t="s">
+      <c r="C67" s="64" t="s">
         <v>41</v>
       </c>
       <c r="D67" s="6" t="s">
@@ -7542,8 +7542,8 @@
       <c r="CF67" s="3"/>
     </row>
     <row r="68" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B68" s="72"/>
-      <c r="C68" s="72"/>
+      <c r="B68" s="74"/>
+      <c r="C68" s="74"/>
       <c r="D68" s="6" t="s">
         <v>5</v>
       </c>
@@ -7629,10 +7629,10 @@
       <c r="CF68" s="3"/>
     </row>
     <row r="69" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B69" s="62">
+      <c r="B69" s="64">
         <v>25</v>
       </c>
-      <c r="C69" s="62" t="s">
+      <c r="C69" s="64" t="s">
         <v>42</v>
       </c>
       <c r="D69" s="6" t="s">
@@ -7720,8 +7720,8 @@
       <c r="CF69" s="3"/>
     </row>
     <row r="70" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B70" s="72"/>
-      <c r="C70" s="72"/>
+      <c r="B70" s="74"/>
+      <c r="C70" s="74"/>
       <c r="D70" s="6" t="s">
         <v>5</v>
       </c>
@@ -7807,10 +7807,10 @@
       <c r="CF70" s="3"/>
     </row>
     <row r="71" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B71" s="62">
+      <c r="B71" s="64">
         <v>26</v>
       </c>
-      <c r="C71" s="62" t="s">
+      <c r="C71" s="64" t="s">
         <v>43</v>
       </c>
       <c r="D71" s="6" t="s">
@@ -7898,8 +7898,8 @@
       <c r="CF71" s="3"/>
     </row>
     <row r="72" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="63"/>
-      <c r="C72" s="63"/>
+      <c r="B72" s="65"/>
+      <c r="C72" s="65"/>
       <c r="D72" s="7" t="s">
         <v>5</v>
       </c>
@@ -7985,10 +7985,10 @@
       <c r="CF72" s="3"/>
     </row>
     <row r="73" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B73" s="64" t="s">
+      <c r="B73" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C73" s="65"/>
+      <c r="C73" s="67"/>
       <c r="D73" s="8" t="s">
         <v>4</v>
       </c>
@@ -8074,8 +8074,8 @@
       <c r="CF73" s="20"/>
     </row>
     <row r="74" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="66"/>
-      <c r="C74" s="67"/>
+      <c r="B74" s="68"/>
+      <c r="C74" s="69"/>
       <c r="D74" s="9" t="s">
         <v>5</v>
       </c>
@@ -8248,10 +8248,10 @@
       <c r="CF75" s="21"/>
     </row>
     <row r="76" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B76" s="71">
+      <c r="B76" s="73">
         <v>27</v>
       </c>
-      <c r="C76" s="71" t="s">
+      <c r="C76" s="73" t="s">
         <v>44</v>
       </c>
       <c r="D76" s="5" t="s">
@@ -8339,8 +8339,8 @@
       <c r="CF76" s="42"/>
     </row>
     <row r="77" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="63"/>
-      <c r="C77" s="72"/>
+      <c r="B77" s="65"/>
+      <c r="C77" s="74"/>
       <c r="D77" s="6" t="s">
         <v>5</v>
       </c>
@@ -8365,9 +8365,9 @@
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
       <c r="Y77" s="1"/>
-      <c r="Z77" s="1"/>
-      <c r="AA77" s="1"/>
-      <c r="AB77" s="3"/>
+      <c r="Z77" s="54"/>
+      <c r="AA77" s="54"/>
+      <c r="AB77" s="59"/>
       <c r="AC77" s="4"/>
       <c r="AD77" s="1"/>
       <c r="AE77" s="1"/>
@@ -8426,10 +8426,10 @@
       <c r="CF77" s="3"/>
     </row>
     <row r="78" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B78" s="71">
+      <c r="B78" s="73">
         <v>28</v>
       </c>
-      <c r="C78" s="62" t="s">
+      <c r="C78" s="64" t="s">
         <v>45</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -8464,7 +8464,7 @@
       <c r="AE78" s="1"/>
       <c r="AF78" s="1"/>
       <c r="AG78" s="1"/>
-      <c r="AH78" s="1"/>
+      <c r="AH78" s="41"/>
       <c r="AI78" s="1"/>
       <c r="AJ78" s="3"/>
       <c r="AK78" s="4"/>
@@ -8517,8 +8517,8 @@
       <c r="CF78" s="3"/>
     </row>
     <row r="79" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B79" s="72"/>
-      <c r="C79" s="72"/>
+      <c r="B79" s="74"/>
+      <c r="C79" s="74"/>
       <c r="D79" s="6" t="s">
         <v>5</v>
       </c>
@@ -8604,10 +8604,10 @@
       <c r="CF79" s="3"/>
     </row>
     <row r="80" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B80" s="62">
+      <c r="B80" s="64">
         <v>29</v>
       </c>
-      <c r="C80" s="62" t="s">
+      <c r="C80" s="64" t="s">
         <v>46</v>
       </c>
       <c r="D80" s="6" t="s">
@@ -8695,8 +8695,8 @@
       <c r="CF80" s="42"/>
     </row>
     <row r="81" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="63"/>
-      <c r="C81" s="63"/>
+      <c r="B81" s="65"/>
+      <c r="C81" s="65"/>
       <c r="D81" s="47" t="s">
         <v>5</v>
       </c>
@@ -8707,7 +8707,7 @@
       <c r="I81" s="49"/>
       <c r="J81" s="49"/>
       <c r="K81" s="49"/>
-      <c r="L81" s="99"/>
+      <c r="L81" s="61"/>
       <c r="M81" s="48"/>
       <c r="N81" s="49"/>
       <c r="O81" s="49"/>
@@ -8715,7 +8715,7 @@
       <c r="Q81" s="49"/>
       <c r="R81" s="49"/>
       <c r="S81" s="49"/>
-      <c r="T81" s="99"/>
+      <c r="T81" s="61"/>
       <c r="U81" s="48"/>
       <c r="V81" s="49"/>
       <c r="W81" s="49"/>
@@ -8723,7 +8723,7 @@
       <c r="Y81" s="49"/>
       <c r="Z81" s="49"/>
       <c r="AA81" s="49"/>
-      <c r="AB81" s="50"/>
+      <c r="AB81" s="61"/>
       <c r="AC81" s="48"/>
       <c r="AD81" s="49"/>
       <c r="AE81" s="49"/>
@@ -8782,10 +8782,10 @@
       <c r="CF81" s="50"/>
     </row>
     <row r="82" spans="2:84" x14ac:dyDescent="0.25">
-      <c r="B82" s="64" t="s">
+      <c r="B82" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C82" s="65"/>
+      <c r="C82" s="67"/>
       <c r="D82" s="8" t="s">
         <v>4</v>
       </c>
@@ -8871,8 +8871,8 @@
       <c r="CF82" s="42"/>
     </row>
     <row r="83" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="66"/>
-      <c r="C83" s="67"/>
+      <c r="B83" s="68"/>
+      <c r="C83" s="69"/>
       <c r="D83" s="9" t="s">
         <v>5</v>
       </c>
@@ -8958,26 +8958,26 @@
       <c r="CF83" s="28"/>
     </row>
     <row r="84" spans="2:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="68" t="s">
+      <c r="B84" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="C84" s="69"/>
-      <c r="D84" s="70"/>
+      <c r="C84" s="71"/>
+      <c r="D84" s="72"/>
       <c r="E84" s="55"/>
-      <c r="F84" s="60" t="s">
+      <c r="F84" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="G84" s="61"/>
+      <c r="G84" s="63"/>
       <c r="H84" s="56"/>
-      <c r="I84" s="60" t="s">
+      <c r="I84" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="J84" s="61"/>
+      <c r="J84" s="63"/>
       <c r="K84" s="57"/>
-      <c r="L84" s="60" t="s">
+      <c r="L84" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="M84" s="61"/>
+      <c r="M84" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="83">

</xml_diff>